<commit_message>
Integrated manage courses, manage classes and course assignment with the rest of project
</commit_message>
<xml_diff>
--- a/Documents/Kickoff Talent Skills Spreadsheet.xlsx
+++ b/Documents/Kickoff Talent Skills Spreadsheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28718"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FasiTahir\6th Semester\SPM\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FasiTahir\Eduvance\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB18E076-E23F-420F-BEE0-8683245777D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3346B-C721-4015-9619-47DD3FE82AE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -545,6 +545,12 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="1" applyFill="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -565,12 +571,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="1" applyFill="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="1" applyFill="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -984,7 +984,7 @@
   <dimension ref="A1:AY417"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B3" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1021,13 +1021,13 @@
       <c r="B2" s="6"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
-      <c r="E2" s="27" t="s">
+      <c r="E2" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
@@ -1043,12 +1043,12 @@
       <c r="E3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="29" t="s">
+      <c r="F3" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="29"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
@@ -1062,12 +1062,12 @@
       <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="32" t="s">
         <v>71</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
       <c r="J4" s="6"/>
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
@@ -1200,16 +1200,16 @@
         <v>4</v>
       </c>
       <c r="D7" s="10"/>
-      <c r="E7" s="32" t="s">
+      <c r="E7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="32" t="s">
+      <c r="F7" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G7" s="32" t="s">
+      <c r="G7" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="32">
+      <c r="H7" s="25">
         <v>2</v>
       </c>
       <c r="I7" s="19">
@@ -1267,16 +1267,16 @@
         <v>5</v>
       </c>
       <c r="D8" s="10"/>
-      <c r="E8" s="31" t="s">
+      <c r="E8" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="H8" s="31">
+      <c r="H8" s="24">
         <v>2</v>
       </c>
       <c r="I8" s="19">
@@ -1334,16 +1334,16 @@
         <v>6</v>
       </c>
       <c r="D9" s="10"/>
-      <c r="E9" s="32" t="s">
+      <c r="E9" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="32" t="s">
+      <c r="G9" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="H9" s="32">
+      <c r="H9" s="25">
         <v>1</v>
       </c>
       <c r="I9" s="19">
@@ -1401,16 +1401,16 @@
         <v>7</v>
       </c>
       <c r="D10" s="10"/>
-      <c r="E10" s="31" t="s">
+      <c r="E10" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G10" s="31" t="s">
+      <c r="G10" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="H10" s="31">
+      <c r="H10" s="24">
         <v>2</v>
       </c>
       <c r="I10" s="19">
@@ -1464,16 +1464,16 @@
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
-      <c r="E11" s="32" t="s">
+      <c r="E11" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="H11" s="32">
+      <c r="H11" s="25">
         <v>1</v>
       </c>
       <c r="I11" s="19">
@@ -1527,16 +1527,16 @@
       <c r="B12" s="12"/>
       <c r="C12" s="12"/>
       <c r="D12" s="6"/>
-      <c r="E12" s="31" t="s">
+      <c r="E12" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="H12" s="31">
+      <c r="H12" s="24">
         <v>2</v>
       </c>
       <c r="I12" s="19">
@@ -1587,21 +1587,21 @@
     </row>
     <row r="13" spans="1:51" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="24"/>
+      <c r="C13" s="26"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="32" t="s">
+      <c r="E13" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="32" t="s">
+      <c r="G13" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="H13" s="32">
+      <c r="H13" s="25">
         <v>2.5</v>
       </c>
       <c r="I13" s="19">
@@ -1652,19 +1652,19 @@
     </row>
     <row r="14" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="24"/>
-      <c r="C14" s="24"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="6"/>
-      <c r="E14" s="31" t="s">
+      <c r="E14" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="31">
+      <c r="H14" s="24">
         <v>2.5</v>
       </c>
       <c r="I14" s="19">
@@ -1715,19 +1715,19 @@
     </row>
     <row r="15" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="24"/>
-      <c r="C15" s="24"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="6"/>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G15" s="32" t="s">
+      <c r="G15" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="H15" s="32">
+      <c r="H15" s="25">
         <v>1</v>
       </c>
       <c r="I15" s="19">
@@ -1778,21 +1778,21 @@
     </row>
     <row r="16" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="28"/>
       <c r="D16" s="6"/>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="31">
+      <c r="H16" s="24">
         <v>2.5</v>
       </c>
       <c r="I16" s="19">
@@ -1845,19 +1845,19 @@
     </row>
     <row r="17" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="6"/>
-      <c r="E17" s="32" t="s">
+      <c r="E17" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="32">
+      <c r="H17" s="25">
         <v>1.5</v>
       </c>
       <c r="I17" s="19">
@@ -1908,19 +1908,19 @@
     </row>
     <row r="18" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
       <c r="D18" s="6"/>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="H18" s="31">
+      <c r="H18" s="24">
         <v>2</v>
       </c>
       <c r="I18" s="19">
@@ -1971,19 +1971,19 @@
     </row>
     <row r="19" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
       <c r="D19" s="6"/>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F19" s="32" t="s">
+      <c r="F19" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G19" s="32" t="s">
+      <c r="G19" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="H19" s="32">
+      <c r="H19" s="25">
         <v>2</v>
       </c>
       <c r="I19" s="19">
@@ -2034,19 +2034,19 @@
     </row>
     <row r="20" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="6"/>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="H20" s="31">
+      <c r="H20" s="24">
         <v>2</v>
       </c>
       <c r="I20" s="19">
@@ -2097,19 +2097,19 @@
     </row>
     <row r="21" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
       <c r="D21" s="6"/>
-      <c r="E21" s="32" t="s">
+      <c r="E21" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="32" t="s">
+      <c r="G21" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="H21" s="32">
+      <c r="H21" s="25">
         <v>1.5</v>
       </c>
       <c r="I21" s="19">
@@ -2160,19 +2160,19 @@
     </row>
     <row r="22" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
       <c r="D22" s="6"/>
-      <c r="E22" s="31" t="s">
+      <c r="E22" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="H22" s="31">
+      <c r="H22" s="24">
         <v>0</v>
       </c>
       <c r="I22" s="19">
@@ -2223,19 +2223,19 @@
     </row>
     <row r="23" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
       <c r="D23" s="6"/>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="32" t="s">
+      <c r="G23" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="H23" s="32">
+      <c r="H23" s="25">
         <v>2.5</v>
       </c>
       <c r="I23" s="19">
@@ -2286,19 +2286,19 @@
     </row>
     <row r="24" spans="1:51" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
       <c r="D24" s="6"/>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="H24" s="31">
+      <c r="H24" s="24">
         <v>2</v>
       </c>
       <c r="I24" s="19">
@@ -2351,16 +2351,16 @@
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="32" t="s">
+      <c r="F25" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="32" t="s">
+      <c r="G25" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="H25" s="32">
+      <c r="H25" s="25">
         <v>1.5</v>
       </c>
       <c r="I25" s="19">
@@ -2411,16 +2411,16 @@
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
       <c r="D26" s="6"/>
-      <c r="E26" s="31" t="s">
+      <c r="E26" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="H26" s="31">
+      <c r="H26" s="24">
         <v>2</v>
       </c>
       <c r="I26" s="19">
@@ -2471,16 +2471,16 @@
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G27" s="32" t="s">
+      <c r="G27" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="H27" s="32">
+      <c r="H27" s="25">
         <v>3</v>
       </c>
       <c r="I27" s="19">
@@ -2531,16 +2531,16 @@
       <c r="B28" s="6"/>
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="31">
+      <c r="H28" s="24">
         <v>2</v>
       </c>
       <c r="I28" s="19">
@@ -2593,16 +2593,16 @@
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
       <c r="D29" s="6"/>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="F29" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G29" s="32" t="s">
+      <c r="G29" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="H29" s="32">
+      <c r="H29" s="25">
         <v>2.5</v>
       </c>
       <c r="I29" s="19">
@@ -2653,16 +2653,16 @@
       <c r="B30" s="6"/>
       <c r="C30" s="6"/>
       <c r="D30" s="6"/>
-      <c r="E30" s="31" t="s">
+      <c r="E30" s="24" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="31">
+      <c r="H30" s="24">
         <v>0.5</v>
       </c>
       <c r="I30" s="19">
@@ -2713,16 +2713,16 @@
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
       <c r="D31" s="6"/>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G31" s="32" t="s">
+      <c r="G31" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="25">
         <v>1</v>
       </c>
       <c r="I31" s="19">
@@ -2773,16 +2773,16 @@
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="6"/>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="H32" s="31">
+      <c r="H32" s="24">
         <v>2</v>
       </c>
       <c r="I32" s="19">
@@ -2832,16 +2832,16 @@
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="32" t="s">
+      <c r="E33" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="G33" s="32" t="s">
+      <c r="G33" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="H33" s="32">
+      <c r="H33" s="25">
         <v>1.5</v>
       </c>
       <c r="I33" s="19">
@@ -2890,16 +2890,16 @@
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="H34" s="31">
+      <c r="H34" s="24">
         <v>1</v>
       </c>
       <c r="I34" s="19">
@@ -2948,16 +2948,16 @@
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="32" t="s">
+      <c r="E35" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F35" s="32" t="s">
+      <c r="F35" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G35" s="32" t="s">
+      <c r="G35" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H35" s="32">
+      <c r="H35" s="25">
         <v>2.5</v>
       </c>
       <c r="I35" s="19">
@@ -3006,16 +3006,16 @@
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="31" t="s">
+      <c r="E36" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="H36" s="31">
+      <c r="H36" s="24">
         <v>2.5</v>
       </c>
       <c r="I36" s="19">
@@ -3064,16 +3064,16 @@
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="32" t="s">
+      <c r="E37" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F37" s="32" t="s">
+      <c r="F37" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="G37" s="32" t="s">
+      <c r="G37" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="H37" s="32">
+      <c r="H37" s="25">
         <v>2</v>
       </c>
       <c r="I37" s="19">
@@ -3122,16 +3122,16 @@
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="31" t="s">
+      <c r="F38" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="H38" s="31">
+      <c r="H38" s="24">
         <v>0.5</v>
       </c>
       <c r="I38" s="19">
@@ -3180,16 +3180,16 @@
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="32" t="s">
+      <c r="E39" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G39" s="32" t="s">
+      <c r="G39" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H39" s="32">
+      <c r="H39" s="25">
         <v>0.5</v>
       </c>
       <c r="I39" s="19">
@@ -3238,16 +3238,16 @@
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="31" t="s">
+      <c r="E40" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="H40" s="31">
+      <c r="H40" s="24">
         <v>0.5</v>
       </c>
       <c r="I40" s="19">
@@ -3296,16 +3296,16 @@
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="32" t="s">
+      <c r="E41" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="F41" s="32" t="s">
+      <c r="F41" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G41" s="32" t="s">
+      <c r="G41" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="H41" s="32">
+      <c r="H41" s="25">
         <v>2.5</v>
       </c>
       <c r="I41" s="19">
@@ -3354,16 +3354,16 @@
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="H42" s="31">
+      <c r="H42" s="24">
         <v>0.5</v>
       </c>
       <c r="I42" s="19">
@@ -3412,16 +3412,16 @@
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="32" t="s">
+      <c r="E43" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F43" s="32" t="s">
+      <c r="F43" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="G43" s="32" t="s">
+      <c r="G43" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="H43" s="32">
+      <c r="H43" s="25">
         <v>0.5</v>
       </c>
       <c r="I43" s="19">
@@ -3470,16 +3470,16 @@
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="31" t="s">
+      <c r="E44" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="H44" s="31">
+      <c r="H44" s="24">
         <v>0.5</v>
       </c>
       <c r="I44" s="19">
@@ -3528,16 +3528,16 @@
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="32" t="s">
+      <c r="E45" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F45" s="32" t="s">
+      <c r="F45" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="G45" s="32" t="s">
+      <c r="G45" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="H45" s="32">
+      <c r="H45" s="25">
         <v>0.5</v>
       </c>
       <c r="I45" s="19">
@@ -3586,16 +3586,16 @@
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="G46" s="31" t="s">
+      <c r="G46" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="H46" s="31">
+      <c r="H46" s="24">
         <v>0.5</v>
       </c>
       <c r="I46" s="19">
@@ -22211,21 +22211,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010063BAC33E40A8AB4AB9A126D298799E78" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="393e3809860021ea4b53ed9d1e2ad736">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9926c504-9366-4d27-ba67-e7df4b72c3ca" xmlns:ns4="675b2d5a-2a5b-4198-b316-84224b1699b9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94008880fd668028e4b73c345dde1642" ns3:_="" ns4:_="">
     <xsd:import namespace="9926c504-9366-4d27-ba67-e7df4b72c3ca"/>
@@ -22442,32 +22427,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC69FD84-4722-485B-95F5-B25971BB4485}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="675b2d5a-2a5b-4198-b316-84224b1699b9"/>
-    <ds:schemaRef ds:uri="9926c504-9366-4d27-ba67-e7df4b72c3ca"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8166D80B-5C7E-4401-9B25-09A4D3E293DD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EED16D48-9510-40B0-BBC1-A62A264ED743}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -22484,4 +22459,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8166D80B-5C7E-4401-9B25-09A4D3E293DD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC69FD84-4722-485B-95F5-B25971BB4485}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="675b2d5a-2a5b-4198-b316-84224b1699b9"/>
+    <ds:schemaRef ds:uri="9926c504-9366-4d27-ba67-e7df4b72c3ca"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>